<commit_message>
add protect modify cell border style for table data
</commit_message>
<xml_diff>
--- a/AsposeDemo/AsposeDemo/ReportTemplates/ReportTemplate.xlsx
+++ b/AsposeDemo/AsposeDemo/ReportTemplates/ReportTemplate.xlsx
@@ -474,9 +474,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>